<commit_message>
Address issues from QA log
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_COM-DTB.xlsx
+++ b/SubRES_TMPL/SubRes_COM-DTB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63099A-4641-427C-8E6E-0B76A86F1B9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22105B94-5D65-4342-941D-C03902D02B53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="19" r:id="rId1"/>
@@ -4381,7 +4381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="711">
   <si>
     <t>Max. capacity factor</t>
   </si>
@@ -7079,7 +7079,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7692,6 +7692,18 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -10130,8 +10142,8 @@
   </sheetPr>
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10491,9 +10503,6 @@
       <c r="AF6" t="s">
         <v>455</v>
       </c>
-      <c r="AG6" t="s">
-        <v>309</v>
-      </c>
       <c r="AJ6" t="str">
         <f>Raw_CCHP!A3</f>
         <v>CHPCOMFCHH2110</v>
@@ -10606,9 +10615,7 @@
       <c r="AF7" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG7" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG7" s="234"/>
       <c r="AJ7" s="234" t="str">
         <f>Raw_CCHP!A4</f>
         <v>CHPCOMICBGS101</v>
@@ -10721,9 +10728,7 @@
       <c r="AF8" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG8" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG8" s="234"/>
       <c r="AJ8" s="234" t="str">
         <f>Raw_CCHP!A5</f>
         <v>CHPCOMICBGS201</v>
@@ -10836,9 +10841,7 @@
       <c r="AF9" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG9" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG9" s="234"/>
       <c r="AJ9" s="234" t="str">
         <f>Raw_CCHP!A6</f>
         <v>CHPCOMICDME101</v>
@@ -10951,9 +10954,7 @@
       <c r="AF10" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG10" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG10" s="234"/>
       <c r="AJ10" s="234" t="str">
         <f>Raw_CCHP!A7</f>
         <v>CHPCOMICDME201</v>
@@ -11066,9 +11067,7 @@
       <c r="AF11" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG11" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG11" s="234"/>
       <c r="AJ11" s="234" t="str">
         <f>Raw_CCHP!A8</f>
         <v>CHPCOMICGAS101</v>
@@ -11181,9 +11180,7 @@
       <c r="AF12" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG12" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG12" s="234"/>
       <c r="AJ12" s="234" t="str">
         <f>Raw_CCHP!A9</f>
         <v>CHPCOMICGAS201</v>
@@ -11296,9 +11293,7 @@
       <c r="AF13" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG13" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG13" s="234"/>
       <c r="AJ13" s="234" t="str">
         <f>Raw_CCHP!A10</f>
         <v>CHPCOMICGAS301</v>
@@ -11411,9 +11406,7 @@
       <c r="AF14" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG14" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG14" s="234"/>
       <c r="AJ14" s="234" t="str">
         <f>Raw_CCHP!A11</f>
         <v>CHPCOMICOIL101</v>
@@ -11526,9 +11519,7 @@
       <c r="AF15" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG15" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG15" s="234"/>
       <c r="AJ15" s="234" t="str">
         <f>Raw_CCHP!A12</f>
         <v>CHPCOMICOIL201</v>
@@ -11641,9 +11632,7 @@
       <c r="AF16" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG16" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG16" s="234"/>
       <c r="AJ16" s="234" t="str">
         <f>Raw_CCHP!A13</f>
         <v>CHPCOMICOIL301</v>
@@ -11765,9 +11754,7 @@
       <c r="AF17" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG17" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG17" s="234"/>
       <c r="AJ17" s="234" t="str">
         <f>Raw_CCHP!A14</f>
         <v>CHPCOMMFBGS110</v>
@@ -11880,9 +11867,7 @@
       <c r="AF18" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG18" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG18" s="234"/>
       <c r="AJ18" s="234" t="str">
         <f>Raw_CCHP!A15</f>
         <v>CHPCOMMFGAS101</v>
@@ -12004,9 +11989,7 @@
       <c r="AF19" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG19" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG19" s="234"/>
       <c r="AJ19" s="234" t="str">
         <f>Raw_CCHP!A16</f>
         <v>CHPCOMSFBGS110</v>
@@ -12128,9 +12111,7 @@
       <c r="AF20" s="234" t="s">
         <v>455</v>
       </c>
-      <c r="AG20" s="234" t="s">
-        <v>309</v>
-      </c>
+      <c r="AG20" s="234"/>
       <c r="AJ20" s="234" t="str">
         <f>Raw_CCHP!A17</f>
         <v>CHPCOMSFGAS101</v>
@@ -12178,7 +12159,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13834,8 +13815,8 @@
   </sheetPr>
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14128,7 +14109,7 @@
         <v>483</v>
       </c>
       <c r="V6" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C6,3)&amp;" "&amp;AC6</f>
+        <f t="shared" ref="V6:V20" si="0">"New commercial - CS Space Heat "&amp;RIGHT(C6,3)&amp;" "&amp;AC6</f>
         <v>New commercial - CS Space Heat ELC Electric radiator</v>
       </c>
       <c r="W6" s="47" t="s">
@@ -14144,11 +14125,11 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="str">
-        <f t="shared" ref="A7:A43" si="0">U7</f>
+        <f t="shared" ref="A7:A43" si="1">U7</f>
         <v>CHCSELC_02_Boi</v>
       </c>
       <c r="B7" s="66" t="str">
-        <f t="shared" ref="B7:B43" si="1">V7</f>
+        <f t="shared" ref="B7:B43" si="2">V7</f>
         <v>New commercial - CS Space Heat ELC Electric boiler</v>
       </c>
       <c r="C7" s="67" t="s">
@@ -14216,7 +14197,7 @@
         <v>484</v>
       </c>
       <c r="V7" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C7,3)&amp;" "&amp;AC7</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Electric boiler</v>
       </c>
       <c r="W7" s="47" t="s">
@@ -14232,11 +14213,11 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_03_HP</v>
       </c>
       <c r="B8" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Air heat pump with electric boiler</v>
       </c>
       <c r="C8" s="67" t="s">
@@ -14304,7 +14285,7 @@
         <v>485</v>
       </c>
       <c r="V8" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C8,3)&amp;" "&amp;AC8</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Air heat pump with electric boiler</v>
       </c>
       <c r="W8" s="47" t="s">
@@ -14321,11 +14302,11 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_04_DHP</v>
       </c>
       <c r="B9" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -14393,7 +14374,7 @@
         <v>486</v>
       </c>
       <c r="V9" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C9,3)&amp;" "&amp;AC9</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W9" s="47" t="s">
@@ -14410,11 +14391,11 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_05_HP</v>
       </c>
       <c r="B10" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Adv Air heat pump with electric boiler</v>
       </c>
       <c r="C10" s="67" t="s">
@@ -14482,7 +14463,7 @@
         <v>487</v>
       </c>
       <c r="V10" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C10,3)&amp;" "&amp;AC10</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Adv Air heat pump with electric boiler</v>
       </c>
       <c r="W10" s="47" t="s">
@@ -14498,11 +14479,11 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_06_DHP</v>
       </c>
       <c r="B11" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Adv Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C11" s="67" t="s">
@@ -14570,7 +14551,7 @@
         <v>488</v>
       </c>
       <c r="V11" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C11,3)&amp;" "&amp;AC11</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Adv Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W11" s="47" t="s">
@@ -14594,11 +14575,11 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_07_HP</v>
       </c>
       <c r="B12" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Ground heat pump with electric boiler</v>
       </c>
       <c r="C12" s="67" t="s">
@@ -14666,7 +14647,7 @@
         <v>489</v>
       </c>
       <c r="V12" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C12,3)&amp;" "&amp;AC12</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Ground heat pump with electric boiler</v>
       </c>
       <c r="W12" s="47" t="s">
@@ -14690,11 +14671,11 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSELC_08_DHP</v>
       </c>
       <c r="B13" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat ELC Ground heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C13" s="67" t="s">
@@ -14762,7 +14743,7 @@
         <v>490</v>
       </c>
       <c r="V13" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C13,3)&amp;" "&amp;AC13</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat ELC Ground heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W13" s="47" t="s">
@@ -14786,11 +14767,11 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>*CHCSFCH_01</v>
       </c>
       <c r="B14" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat HET FC output to Heat demand</v>
       </c>
       <c r="C14" s="238" t="s">
@@ -14858,7 +14839,7 @@
         <v>424</v>
       </c>
       <c r="V14" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C14,3)&amp;" "&amp;AC14</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat HET FC output to Heat demand</v>
       </c>
       <c r="W14" s="47" t="s">
@@ -14882,11 +14863,11 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_01_Boi</v>
       </c>
       <c r="B15" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler</v>
       </c>
       <c r="C15" s="67" t="s">
@@ -14954,7 +14935,7 @@
         <v>491</v>
       </c>
       <c r="V15" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C15,3)&amp;" "&amp;AC15</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler</v>
       </c>
       <c r="W15" s="47" t="s">
@@ -14978,11 +14959,11 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_02_DBoi</v>
       </c>
       <c r="B16" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler.HeatHotwater</v>
       </c>
       <c r="C16" s="67" t="s">
@@ -15050,7 +15031,7 @@
         <v>492</v>
       </c>
       <c r="V16" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C16,3)&amp;" "&amp;AC16</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler.HeatHotwater</v>
       </c>
       <c r="W16" s="47" t="s">
@@ -15066,11 +15047,11 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_03_Boi</v>
       </c>
       <c r="B17" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler condensing</v>
       </c>
       <c r="C17" s="67" t="s">
@@ -15138,7 +15119,7 @@
         <v>493</v>
       </c>
       <c r="V17" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C17,3)&amp;" "&amp;AC17</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler condensing</v>
       </c>
       <c r="W17" s="47" t="s">
@@ -15154,11 +15135,11 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_04_DBoi</v>
       </c>
       <c r="B18" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler condensing.HeatHotwater</v>
       </c>
       <c r="C18" s="67" t="s">
@@ -15226,7 +15207,7 @@
         <v>494</v>
       </c>
       <c r="V18" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C18,3)&amp;" "&amp;AC18</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas boiler condensing.HeatHotwater</v>
       </c>
       <c r="W18" s="47" t="s">
@@ -15242,11 +15223,11 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_05_HP</v>
       </c>
       <c r="B19" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas air heat pump</v>
       </c>
       <c r="C19" s="67" t="s">
@@ -15314,7 +15295,7 @@
         <v>495</v>
       </c>
       <c r="V19" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C19,3)&amp;" "&amp;AC19</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas air heat pump</v>
       </c>
       <c r="W19" s="47" t="s">
@@ -15330,11 +15311,11 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSGAS_06_DHP</v>
       </c>
       <c r="B20" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat GAS Natural gas air heat pump.HeatCool</v>
       </c>
       <c r="C20" s="67" t="s">
@@ -15402,7 +15383,7 @@
         <v>496</v>
       </c>
       <c r="V20" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C20,3)&amp;" "&amp;AC20</f>
+        <f t="shared" si="0"/>
         <v>New commercial - CS Space Heat GAS Natural gas air heat pump.HeatCool</v>
       </c>
       <c r="W20" s="47" t="s">
@@ -15418,11 +15399,11 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSLPG_01_Boi</v>
       </c>
       <c r="B21" s="66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat LPG boiler</v>
       </c>
       <c r="C21" s="66" t="s">
@@ -15506,11 +15487,11 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSLPG_02_DBoi</v>
       </c>
       <c r="B22" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat LPG boiler.HeatHotwater</v>
       </c>
       <c r="C22" s="66" t="s">
@@ -15578,7 +15559,7 @@
         <v>498</v>
       </c>
       <c r="V22" s="47" t="str">
-        <f t="shared" ref="V22" si="2">"New commercial - CS Space Heat "&amp;AC22</f>
+        <f t="shared" ref="V22" si="3">"New commercial - CS Space Heat "&amp;AC22</f>
         <v>New commercial - CS Space Heat LPG boiler.HeatHotwater</v>
       </c>
       <c r="W22" s="47" t="s">
@@ -15594,11 +15575,11 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSLPG_04_DHP</v>
       </c>
       <c r="B23" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat LPG LPG air heat pump.HeatCool</v>
       </c>
       <c r="C23" s="67" t="s">
@@ -15666,7 +15647,7 @@
         <v>499</v>
       </c>
       <c r="V23" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C23,3)&amp;" "&amp;AC23</f>
+        <f t="shared" ref="V23:V31" si="4">"New commercial - CS Space Heat "&amp;RIGHT(C23,3)&amp;" "&amp;AC23</f>
         <v>New commercial - CS Space Heat LPG LPG air heat pump.HeatCool</v>
       </c>
       <c r="W23" s="47" t="s">
@@ -15682,11 +15663,11 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSHET_01_DH</v>
       </c>
       <c r="B24" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat HET District heat exchanger.HeatHotwater</v>
       </c>
       <c r="C24" s="67" t="s">
@@ -15754,7 +15735,7 @@
         <v>500</v>
       </c>
       <c r="V24" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C24,3)&amp;" "&amp;AC24</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat HET District heat exchanger.HeatHotwater</v>
       </c>
       <c r="W24" s="47" t="s">
@@ -15770,11 +15751,11 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSOIL_01_Boi</v>
       </c>
       <c r="B25" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat OIL Oil boiler</v>
       </c>
       <c r="C25" s="67" t="s">
@@ -15842,7 +15823,7 @@
         <v>501</v>
       </c>
       <c r="V25" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C25,3)&amp;" "&amp;AC25</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat OIL Oil boiler</v>
       </c>
       <c r="W25" s="47" t="s">
@@ -15858,11 +15839,11 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSOIL_02_DBoi</v>
       </c>
       <c r="B26" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat OIL Oil boiler.HeatHotwater</v>
       </c>
       <c r="C26" s="67" t="s">
@@ -15930,7 +15911,7 @@
         <v>502</v>
       </c>
       <c r="V26" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C26,3)&amp;" "&amp;AC26</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat OIL Oil boiler.HeatHotwater</v>
       </c>
       <c r="W26" s="47" t="s">
@@ -15946,11 +15927,11 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSOIL_03_DBoi</v>
       </c>
       <c r="B27" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat OIL Oil boiler condensing.HeatHotwater</v>
       </c>
       <c r="C27" s="67" t="s">
@@ -16018,7 +15999,7 @@
         <v>503</v>
       </c>
       <c r="V27" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C27,3)&amp;" "&amp;AC27</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat OIL Oil boiler condensing.HeatHotwater</v>
       </c>
       <c r="W27" s="47" t="s">
@@ -16034,11 +16015,11 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSSOL_01_EBkp</v>
       </c>
       <c r="B28" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat SOL Solar collector with electric backup.HeatHotwater</v>
       </c>
       <c r="C28" s="67" t="s">
@@ -16106,7 +16087,7 @@
         <v>504</v>
       </c>
       <c r="V28" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C28,3)&amp;" "&amp;AC28</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat SOL Solar collector with electric backup.HeatHotwater</v>
       </c>
       <c r="W28" s="47" t="s">
@@ -16122,11 +16103,11 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSSOL_02_DBkp</v>
       </c>
       <c r="B29" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat SOL Solar collector with diesel backup.HeatHotwater</v>
       </c>
       <c r="C29" s="67" t="s">
@@ -16194,7 +16175,7 @@
         <v>516</v>
       </c>
       <c r="V29" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C29,3)&amp;" "&amp;AC29</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat SOL Solar collector with diesel backup.HeatHotwater</v>
       </c>
       <c r="W29" s="47" t="s">
@@ -16210,11 +16191,11 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSSOL_03_GBkp</v>
       </c>
       <c r="B30" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat SOL Solar collector with gas backup.HeatHotwater</v>
       </c>
       <c r="C30" s="67" t="s">
@@ -16282,7 +16263,7 @@
         <v>517</v>
       </c>
       <c r="V30" s="47" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C30,3)&amp;" "&amp;AC30</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat SOL Solar collector with gas backup.HeatHotwater</v>
       </c>
       <c r="W30" s="47" t="s">
@@ -16298,11 +16279,11 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHCSBIO_01_DBoi</v>
       </c>
       <c r="B31" s="73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - CS Space Heat BIO Wood-pellets boiler.HeatHotwater</v>
       </c>
       <c r="C31" s="73" t="s">
@@ -16371,7 +16352,7 @@
         <v>505</v>
       </c>
       <c r="V31" s="97" t="str">
-        <f>"New commercial - CS Space Heat "&amp;RIGHT(C31,3)&amp;" "&amp;AC31</f>
+        <f t="shared" si="4"/>
         <v>New commercial - CS Space Heat BIO Wood-pellets boiler.HeatHotwater</v>
       </c>
       <c r="W31" s="97" t="s">
@@ -16610,74 +16591,74 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_01_Rad</v>
       </c>
       <c r="B37" s="64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Electric radiator</v>
       </c>
       <c r="C37" s="64" t="str">
-        <f t="shared" ref="C37:C62" si="3">C6</f>
+        <f t="shared" ref="C37:C62" si="5">C6</f>
         <v>COMELC</v>
       </c>
       <c r="D37" s="78" t="s">
         <v>320</v>
       </c>
       <c r="E37" s="79">
-        <f t="shared" ref="E37:E62" si="4">IF(E6=0,"",E6)</f>
+        <f t="shared" ref="E37:E62" si="6">IF(E6=0,"",E6)</f>
         <v>0.93</v>
       </c>
       <c r="F37" s="79" t="str">
-        <f t="shared" ref="F37:H62" si="5">IF(F6="","",F6)</f>
+        <f t="shared" ref="F37:H62" si="7">IF(F6="","",F6)</f>
         <v/>
       </c>
       <c r="G37" s="79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H37" s="79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I37" s="80">
-        <f t="shared" ref="I37:O43" si="6">I6</f>
+        <f t="shared" ref="I37:O43" si="8">I6</f>
         <v>2019</v>
       </c>
       <c r="J37" s="81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="K37" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L37" s="83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M37" s="80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N37" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O37" s="79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P37" s="84" t="str">
-        <f t="shared" ref="P37:R43" si="7">IF(P6=0,"",P6)</f>
+        <f t="shared" ref="P37:R43" si="9">IF(P6=0,"",P6)</f>
         <v/>
       </c>
       <c r="Q37" s="84" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R37" s="84" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T37" s="47" t="s">
@@ -16687,7 +16668,7 @@
         <v>460</v>
       </c>
       <c r="V37" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C6,3)&amp;" "&amp;AC6</f>
+        <f t="shared" ref="V37:V62" si="10">"New commercial - PS Space Heat "&amp;RIGHT(C6,3)&amp;" "&amp;AC6</f>
         <v>New commercial - PS Space Heat ELC Electric radiator</v>
       </c>
       <c r="W37" s="47" t="s">
@@ -16701,81 +16682,81 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_02_Boi</v>
       </c>
       <c r="B38" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Electric boiler</v>
       </c>
       <c r="C38" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMELC</v>
       </c>
       <c r="D38" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E38" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.88349999999999995</v>
       </c>
       <c r="F38" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G38" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H38" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I38" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J38" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>220</v>
       </c>
       <c r="K38" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="L38" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M38" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N38" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O38" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P38" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Q38" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R38" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U38" s="158" t="s">
         <v>461</v>
       </c>
       <c r="V38" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C7,3)&amp;" "&amp;AC7</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Electric boiler</v>
       </c>
       <c r="W38" s="47" t="s">
@@ -16789,81 +16770,81 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_03_HP</v>
       </c>
       <c r="B39" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Air heat pump with electric boiler</v>
       </c>
       <c r="C39" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D39" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E39" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93</v>
       </c>
       <c r="F39" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G39" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H39" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I39" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J39" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>600</v>
       </c>
       <c r="K39" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="L39" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M39" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N39" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O39" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P39" s="90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.69696969696969702</v>
       </c>
       <c r="Q39" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R39" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U39" s="158" t="s">
         <v>468</v>
       </c>
       <c r="V39" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C8,3)&amp;" "&amp;AC8</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Air heat pump with electric boiler</v>
       </c>
       <c r="W39" s="47" t="s">
@@ -16877,81 +16858,81 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_04_DHP</v>
       </c>
       <c r="B40" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C40" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D40" s="86" t="s">
         <v>326</v>
       </c>
       <c r="E40" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F40" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G40" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H40" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I40" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J40" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>600</v>
       </c>
       <c r="K40" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="L40" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M40" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N40" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O40" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P40" s="90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.69696969696969702</v>
       </c>
       <c r="Q40" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R40" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U40" s="158" t="s">
         <v>469</v>
       </c>
       <c r="V40" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C9,3)&amp;" "&amp;AC9</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W40" s="47" t="s">
@@ -16965,81 +16946,81 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_05_HP</v>
       </c>
       <c r="B41" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Adv Air heat pump with electric boiler</v>
       </c>
       <c r="C41" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D41" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E41" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93</v>
       </c>
       <c r="F41" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G41" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H41" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I41" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J41" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1200</v>
       </c>
       <c r="K41" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="L41" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M41" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N41" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O41" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P41" s="90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.79166666666666696</v>
       </c>
       <c r="Q41" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R41" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U41" s="158" t="s">
         <v>470</v>
       </c>
       <c r="V41" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C10,3)&amp;" "&amp;AC10</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Adv Air heat pump with electric boiler</v>
       </c>
       <c r="W41" s="47" t="s">
@@ -17053,81 +17034,81 @@
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_06_DHP</v>
       </c>
       <c r="B42" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Adv Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C42" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D42" s="86" t="s">
         <v>326</v>
       </c>
       <c r="E42" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F42" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G42" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H42" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I42" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J42" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1200</v>
       </c>
       <c r="K42" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="L42" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M42" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N42" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O42" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P42" s="90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.82758620689655205</v>
       </c>
       <c r="Q42" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R42" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U42" s="158" t="s">
         <v>471</v>
       </c>
       <c r="V42" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C11,3)&amp;" "&amp;AC11</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Adv Air heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W42" s="47" t="s">
@@ -17141,62 +17122,62 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>CHPSELC_07_HP</v>
       </c>
       <c r="B43" s="67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>New commercial - PS Space Heat ELC Ground heat pump with electric boiler</v>
       </c>
       <c r="C43" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D43" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E43" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93</v>
       </c>
       <c r="F43" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G43" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H43" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I43" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="J43" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>700</v>
       </c>
       <c r="K43" s="82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="L43" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M43" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="N43" s="68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O43" s="87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15</v>
       </c>
       <c r="P43" s="90">
@@ -17204,18 +17185,18 @@
         <v>0.8</v>
       </c>
       <c r="Q43" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R43" s="90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U43" s="158" t="s">
         <v>472</v>
       </c>
       <c r="V43" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C12,3)&amp;" "&amp;AC12</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Ground heat pump with electric boiler</v>
       </c>
       <c r="W43" s="47" t="s">
@@ -17229,62 +17210,62 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="86" t="str">
-        <f t="shared" ref="A44:A62" si="8">U44</f>
+        <f t="shared" ref="A44:A62" si="11">U44</f>
         <v>CHPSELC_08_DHP</v>
       </c>
       <c r="B44" s="67" t="str">
-        <f t="shared" ref="B44:B62" si="9">V44</f>
+        <f t="shared" ref="B44:B62" si="12">V44</f>
         <v>New commercial - PS Space Heat ELC Ground heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="C44" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMELC</v>
       </c>
       <c r="D44" s="86" t="s">
         <v>326</v>
       </c>
       <c r="E44" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F44" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G44" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H44" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I44" s="88">
-        <f t="shared" ref="I44:O44" si="10">I13</f>
+        <f t="shared" ref="I44:O44" si="13">I13</f>
         <v>2019</v>
       </c>
       <c r="J44" s="82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>700</v>
       </c>
       <c r="K44" s="82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="L44" s="89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.01</v>
       </c>
       <c r="M44" s="88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="N44" s="68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O44" s="87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.15</v>
       </c>
       <c r="P44" s="90">
@@ -17292,18 +17273,18 @@
         <v>0.8</v>
       </c>
       <c r="Q44" s="90" t="str">
-        <f t="shared" ref="Q44:R44" si="11">IF(Q13=0,"",Q13)</f>
+        <f t="shared" ref="Q44:R44" si="14">IF(Q13=0,"",Q13)</f>
         <v/>
       </c>
       <c r="R44" s="90" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="U44" s="158" t="s">
         <v>473</v>
       </c>
       <c r="V44" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C13,3)&amp;" "&amp;AC13</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat ELC Ground heat pump with electric boiler.HeatCool</v>
       </c>
       <c r="W44" s="47" t="s">
@@ -17317,81 +17298,81 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>*CHPSFCH_01</v>
       </c>
       <c r="B45" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat HET FC output to Heat demand</v>
       </c>
       <c r="C45" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMHET</v>
       </c>
       <c r="D45" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E45" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93</v>
       </c>
       <c r="F45" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G45" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H45" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I45" s="88">
-        <f t="shared" ref="I45:O45" si="12">I14</f>
+        <f t="shared" ref="I45:O45" si="15">I14</f>
         <v>2019</v>
       </c>
       <c r="J45" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
       <c r="K45" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L45" s="89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
       <c r="M45" s="88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="N45" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O45" s="87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.15</v>
       </c>
       <c r="P45" s="90" t="str">
-        <f t="shared" ref="P45:R45" si="13">IF(P14=0,"",P14)</f>
+        <f t="shared" ref="P45:R45" si="16">IF(P14=0,"",P14)</f>
         <v/>
       </c>
       <c r="Q45" s="90" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="R45" s="90" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="U45" s="158" t="s">
         <v>425</v>
       </c>
       <c r="V45" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C14,3)&amp;" "&amp;AC14</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat HET FC output to Heat demand</v>
       </c>
       <c r="W45" s="47" t="s">
@@ -17405,81 +17386,81 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_01_Boi</v>
       </c>
       <c r="B46" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler</v>
       </c>
       <c r="C46" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMGAS</v>
       </c>
       <c r="D46" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E46" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.81840000000000002</v>
       </c>
       <c r="F46" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G46" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H46" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I46" s="88">
-        <f t="shared" ref="I46:O46" si="14">I15</f>
+        <f t="shared" ref="I46:O46" si="17">I15</f>
         <v>2019</v>
       </c>
       <c r="J46" s="82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>109</v>
       </c>
       <c r="K46" s="82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>7.3</v>
       </c>
       <c r="L46" s="89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.01</v>
       </c>
       <c r="M46" s="88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="N46" s="68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O46" s="87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.15</v>
       </c>
       <c r="P46" s="90" t="str">
-        <f t="shared" ref="P46:R46" si="15">IF(P15=0,"",P15)</f>
+        <f t="shared" ref="P46:R46" si="18">IF(P15=0,"",P15)</f>
         <v/>
       </c>
       <c r="Q46" s="90" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="R46" s="90" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="U46" s="158" t="s">
         <v>462</v>
       </c>
       <c r="V46" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C15,3)&amp;" "&amp;AC15</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler</v>
       </c>
       <c r="W46" s="47" t="s">
@@ -17493,81 +17474,81 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_02_DBoi</v>
       </c>
       <c r="B47" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler.HeatHotwater</v>
       </c>
       <c r="C47" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMGAS</v>
       </c>
       <c r="D47" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E47" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F47" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.88349999999999995</v>
       </c>
       <c r="G47" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.59670000000000001</v>
       </c>
       <c r="H47" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I47" s="88">
-        <f t="shared" ref="I47:O47" si="16">I16</f>
+        <f t="shared" ref="I47:O47" si="19">I16</f>
         <v>2019</v>
       </c>
       <c r="J47" s="82">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>119.9</v>
       </c>
       <c r="K47" s="82">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="L47" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.01</v>
       </c>
       <c r="M47" s="88">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>20</v>
       </c>
       <c r="N47" s="68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O47" s="87">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.16</v>
       </c>
       <c r="P47" s="90" t="str">
-        <f t="shared" ref="P47:R47" si="17">IF(P16=0,"",P16)</f>
+        <f t="shared" ref="P47:R47" si="20">IF(P16=0,"",P16)</f>
         <v/>
       </c>
       <c r="Q47" s="90" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="R47" s="90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.6</v>
       </c>
       <c r="U47" s="158" t="s">
         <v>463</v>
       </c>
       <c r="V47" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C16,3)&amp;" "&amp;AC16</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler.HeatHotwater</v>
       </c>
       <c r="W47" s="47" t="s">
@@ -17581,81 +17562,81 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_03_Boi</v>
       </c>
       <c r="B48" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler condensing</v>
       </c>
       <c r="C48" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMGAS</v>
       </c>
       <c r="D48" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E48" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0229999999999999</v>
       </c>
       <c r="F48" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G48" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H48" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I48" s="88">
-        <f t="shared" ref="I48:O48" si="18">I17</f>
+        <f t="shared" ref="I48:O48" si="21">I17</f>
         <v>2019</v>
       </c>
       <c r="J48" s="82">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>256</v>
       </c>
       <c r="K48" s="82">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.3</v>
       </c>
       <c r="L48" s="89">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.01</v>
       </c>
       <c r="M48" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="N48" s="68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O48" s="87">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.15</v>
       </c>
       <c r="P48" s="90" t="str">
-        <f t="shared" ref="P48:R48" si="19">IF(P17=0,"",P17)</f>
+        <f t="shared" ref="P48:R48" si="22">IF(P17=0,"",P17)</f>
         <v/>
       </c>
       <c r="Q48" s="90" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="R48" s="90" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U48" s="158" t="s">
         <v>464</v>
       </c>
       <c r="V48" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C17,3)&amp;" "&amp;AC17</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler condensing</v>
       </c>
       <c r="W48" s="47" t="s">
@@ -17669,81 +17650,81 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_04_DBoi</v>
       </c>
       <c r="B49" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler condensing.HeatHotwater</v>
       </c>
       <c r="C49" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMGAS</v>
       </c>
       <c r="D49" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E49" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F49" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99509999999999998</v>
       </c>
       <c r="G49" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.50467289719626196</v>
       </c>
       <c r="H49" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I49" s="88">
-        <f t="shared" ref="I49:O49" si="20">I18</f>
+        <f t="shared" ref="I49:O49" si="23">I18</f>
         <v>2019</v>
       </c>
       <c r="J49" s="82">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>281.60000000000002</v>
       </c>
       <c r="K49" s="82">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>7.3</v>
       </c>
       <c r="L49" s="89">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="M49" s="88">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="N49" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O49" s="87">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.16</v>
       </c>
       <c r="P49" s="90" t="str">
-        <f t="shared" ref="P49:R49" si="21">IF(P18=0,"",P18)</f>
+        <f t="shared" ref="P49:R49" si="24">IF(P18=0,"",P18)</f>
         <v/>
       </c>
       <c r="Q49" s="90" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R49" s="90">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0.6</v>
       </c>
       <c r="U49" s="158" t="s">
         <v>465</v>
       </c>
       <c r="V49" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C18,3)&amp;" "&amp;AC18</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas boiler condensing.HeatHotwater</v>
       </c>
       <c r="W49" s="47" t="s">
@@ -17757,81 +17738,81 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_05_HP</v>
       </c>
       <c r="B50" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas air heat pump</v>
       </c>
       <c r="C50" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMGAS</v>
       </c>
       <c r="D50" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E50" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.93</v>
       </c>
       <c r="F50" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G50" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H50" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I50" s="88">
-        <f t="shared" ref="I50:O50" si="22">I19</f>
+        <f t="shared" ref="I50:O50" si="25">I19</f>
         <v>2019</v>
       </c>
       <c r="J50" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>509</v>
       </c>
       <c r="K50" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="L50" s="89">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="M50" s="88">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="N50" s="68">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O50" s="87">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0.15</v>
       </c>
       <c r="P50" s="90">
-        <f t="shared" ref="P50:R50" si="23">IF(P19=0,"",P19)</f>
+        <f t="shared" ref="P50:R50" si="26">IF(P19=0,"",P19)</f>
         <v>0.42857142857142899</v>
       </c>
       <c r="Q50" s="90" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="R50" s="90" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="U50" s="158" t="s">
         <v>466</v>
       </c>
       <c r="V50" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C19,3)&amp;" "&amp;AC19</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas air heat pump</v>
       </c>
       <c r="W50" s="47" t="s">
@@ -17845,81 +17826,81 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSGAS_06_DHP</v>
       </c>
       <c r="B51" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat GAS Natural gas air heat pump.HeatCool</v>
       </c>
       <c r="C51" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMGAS</v>
       </c>
       <c r="D51" s="86" t="s">
         <v>326</v>
       </c>
       <c r="E51" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F51" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G51" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H51" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I51" s="88">
-        <f t="shared" ref="I51:O51" si="24">I20</f>
+        <f t="shared" ref="I51:O51" si="27">I20</f>
         <v>2019</v>
       </c>
       <c r="J51" s="82">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>509</v>
       </c>
       <c r="K51" s="82">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>9</v>
       </c>
       <c r="L51" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.01</v>
       </c>
       <c r="M51" s="88">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>20</v>
       </c>
       <c r="N51" s="68">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O51" s="87">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.15</v>
       </c>
       <c r="P51" s="90">
-        <f t="shared" ref="P51:R51" si="25">IF(P20=0,"",P20)</f>
+        <f t="shared" ref="P51:R51" si="28">IF(P20=0,"",P20)</f>
         <v>0.42857142857142899</v>
       </c>
       <c r="Q51" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="R51" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="U51" s="158" t="s">
         <v>467</v>
       </c>
       <c r="V51" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C20,3)&amp;" "&amp;AC20</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat GAS Natural gas air heat pump.HeatCool</v>
       </c>
       <c r="W51" s="47" t="s">
@@ -17933,81 +17914,81 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSLPG_01_Boi</v>
       </c>
       <c r="B52" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat LPG LPG boiler</v>
       </c>
       <c r="C52" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMLPG</v>
       </c>
       <c r="D52" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E52" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.79049999999999998</v>
       </c>
       <c r="F52" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G52" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H52" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I52" s="88">
-        <f t="shared" ref="I52:O52" si="26">I21</f>
+        <f t="shared" ref="I52:O52" si="29">I21</f>
         <v>2019</v>
       </c>
       <c r="J52" s="82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>147</v>
       </c>
       <c r="K52" s="82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>8.5</v>
       </c>
       <c r="L52" s="89">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0.01</v>
       </c>
       <c r="M52" s="88">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="N52" s="68">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O52" s="87">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0.15</v>
       </c>
       <c r="P52" s="90" t="str">
-        <f t="shared" ref="P52:R52" si="27">IF(P21=0,"",P21)</f>
+        <f t="shared" ref="P52:R52" si="30">IF(P21=0,"",P21)</f>
         <v/>
       </c>
       <c r="Q52" s="90" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="R52" s="90" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="U52" s="158" t="s">
         <v>474</v>
       </c>
       <c r="V52" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C21,3)&amp;" "&amp;AC21</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat LPG LPG boiler</v>
       </c>
       <c r="W52" s="47" t="s">
@@ -18020,81 +18001,81 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSLPG_02_DBoi</v>
       </c>
       <c r="B53" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat LPG LPG boiler.HeatHotwater</v>
       </c>
       <c r="C53" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMLPG</v>
       </c>
       <c r="D53" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E53" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F53" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.68262</v>
       </c>
       <c r="G53" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.73569482288828403</v>
       </c>
       <c r="H53" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I53" s="88">
-        <f t="shared" ref="I53:O53" si="28">I22</f>
+        <f t="shared" ref="I53:O53" si="31">I22</f>
         <v>2019</v>
       </c>
       <c r="J53" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>161.69999999999999</v>
       </c>
       <c r="K53" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>1.32</v>
       </c>
       <c r="L53" s="89">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.01</v>
       </c>
       <c r="M53" s="88">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>20</v>
       </c>
       <c r="N53" s="68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O53" s="87">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.16</v>
       </c>
       <c r="P53" s="90" t="str">
-        <f t="shared" ref="P53:R53" si="29">IF(P22=0,"",P22)</f>
+        <f t="shared" ref="P53:R53" si="32">IF(P22=0,"",P22)</f>
         <v/>
       </c>
       <c r="Q53" s="90" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="R53" s="90">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.6</v>
       </c>
       <c r="U53" s="158" t="s">
         <v>475</v>
       </c>
       <c r="V53" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C22,3)&amp;" "&amp;AC22</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat LPG LPG boiler.HeatHotwater</v>
       </c>
       <c r="W53" s="47" t="s">
@@ -18107,81 +18088,81 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSLPG_04_DHP</v>
       </c>
       <c r="B54" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat LPG LPG air heat pump.HeatCool</v>
       </c>
       <c r="C54" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMAMB, COMLPG</v>
       </c>
       <c r="D54" s="86" t="s">
         <v>326</v>
       </c>
       <c r="E54" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F54" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G54" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H54" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I54" s="88">
-        <f t="shared" ref="I54:O54" si="30">I23</f>
+        <f t="shared" ref="I54:O54" si="33">I23</f>
         <v>2019</v>
       </c>
       <c r="J54" s="82">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>600</v>
       </c>
       <c r="K54" s="82">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>7.84</v>
       </c>
       <c r="L54" s="89">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.01</v>
       </c>
       <c r="M54" s="88">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>20</v>
       </c>
       <c r="N54" s="68">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O54" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.15</v>
       </c>
       <c r="P54" s="90">
-        <f t="shared" ref="P54:R54" si="31">IF(P23=0,"",P23)</f>
+        <f t="shared" ref="P54:R54" si="34">IF(P23=0,"",P23)</f>
         <v>0.5</v>
       </c>
       <c r="Q54" s="90" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="R54" s="90" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="U54" s="158" t="s">
         <v>476</v>
       </c>
       <c r="V54" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C23,3)&amp;" "&amp;AC23</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat LPG LPG air heat pump.HeatCool</v>
       </c>
       <c r="W54" s="47" t="s">
@@ -18194,81 +18175,81 @@
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSHET_01_DH</v>
       </c>
       <c r="B55" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat HET District heat exchanger.HeatHotwater</v>
       </c>
       <c r="C55" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMHET</v>
       </c>
       <c r="D55" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E55" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F55" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.88349999999999995</v>
       </c>
       <c r="G55" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
       <c r="H55" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I55" s="88">
-        <f t="shared" ref="I55:O55" si="32">I24</f>
+        <f t="shared" ref="I55:O55" si="35">I24</f>
         <v>2019</v>
       </c>
       <c r="J55" s="82">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>70</v>
       </c>
       <c r="K55" s="82">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="L55" s="89">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.01</v>
       </c>
       <c r="M55" s="88">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>20</v>
       </c>
       <c r="N55" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O55" s="87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.16</v>
       </c>
       <c r="P55" s="90" t="str">
-        <f t="shared" ref="P55:R55" si="33">IF(P24=0,"",P24)</f>
+        <f t="shared" ref="P55:R55" si="36">IF(P24=0,"",P24)</f>
         <v/>
       </c>
       <c r="Q55" s="90" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="R55" s="90">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.6</v>
       </c>
       <c r="U55" s="158" t="s">
         <v>477</v>
       </c>
       <c r="V55" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C24,3)&amp;" "&amp;AC24</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat HET District heat exchanger.HeatHotwater</v>
       </c>
       <c r="W55" s="47" t="s">
@@ -18281,81 +18262,81 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSOIL_01_Boi</v>
       </c>
       <c r="B56" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat OIL Oil boiler</v>
       </c>
       <c r="C56" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMOIL</v>
       </c>
       <c r="D56" s="86" t="s">
         <v>320</v>
       </c>
       <c r="E56" s="87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.67889999999999995</v>
       </c>
       <c r="F56" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G56" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H56" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I56" s="88">
-        <f t="shared" ref="I56:O56" si="34">I25</f>
+        <f t="shared" ref="I56:O56" si="37">I25</f>
         <v>2019</v>
       </c>
       <c r="J56" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>62.45</v>
       </c>
       <c r="K56" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>1.25</v>
       </c>
       <c r="L56" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.01</v>
       </c>
       <c r="M56" s="88">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>20</v>
       </c>
       <c r="N56" s="68">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O56" s="87">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="P56" s="90" t="str">
-        <f t="shared" ref="P56:R56" si="35">IF(P25=0,"",P25)</f>
+        <f t="shared" ref="P56:R56" si="38">IF(P25=0,"",P25)</f>
         <v/>
       </c>
       <c r="Q56" s="90" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="R56" s="90" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="U56" s="158" t="s">
         <v>478</v>
       </c>
       <c r="V56" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C25,3)&amp;" "&amp;AC25</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat OIL Oil boiler</v>
       </c>
       <c r="W56" s="47" t="s">
@@ -18368,81 +18349,81 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSOIL_02_DBoi</v>
       </c>
       <c r="B57" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat OIL Oil boiler.HeatHotwater</v>
       </c>
       <c r="C57" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMOIL</v>
       </c>
       <c r="D57" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E57" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F57" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.79049999999999998</v>
       </c>
       <c r="G57" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.59670000000000001</v>
       </c>
       <c r="H57" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I57" s="88">
-        <f t="shared" ref="I57:O57" si="36">I26</f>
+        <f t="shared" ref="I57:O57" si="39">I26</f>
         <v>2019</v>
       </c>
       <c r="J57" s="82">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>68.694999999999993</v>
       </c>
       <c r="K57" s="82">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="L57" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.01</v>
       </c>
       <c r="M57" s="88">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>20</v>
       </c>
       <c r="N57" s="68">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O57" s="87">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.16</v>
       </c>
       <c r="P57" s="90" t="str">
-        <f t="shared" ref="P57:R57" si="37">IF(P26=0,"",P26)</f>
+        <f t="shared" ref="P57:R57" si="40">IF(P26=0,"",P26)</f>
         <v/>
       </c>
       <c r="Q57" s="90" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="R57" s="90">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.6</v>
       </c>
       <c r="U57" s="158" t="s">
         <v>479</v>
       </c>
       <c r="V57" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C26,3)&amp;" "&amp;AC26</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat OIL Oil boiler.HeatHotwater</v>
       </c>
       <c r="W57" s="47" t="s">
@@ -18455,81 +18436,81 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSOIL_03_DBoi</v>
       </c>
       <c r="B58" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat OIL Oil boiler condensing.HeatHotwater</v>
       </c>
       <c r="C58" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMOIL</v>
       </c>
       <c r="D58" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E58" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F58" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="G58" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.34200000000000003</v>
       </c>
       <c r="H58" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I58" s="88">
-        <f t="shared" ref="I58:O58" si="38">I27</f>
+        <f t="shared" ref="I58:O58" si="41">I27</f>
         <v>2019</v>
       </c>
       <c r="J58" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>279</v>
       </c>
       <c r="K58" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>4</v>
       </c>
       <c r="L58" s="89">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.01</v>
       </c>
       <c r="M58" s="88">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>20</v>
       </c>
       <c r="N58" s="68">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O58" s="87">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.16</v>
       </c>
       <c r="P58" s="90" t="str">
-        <f t="shared" ref="P58:R58" si="39">IF(P27=0,"",P27)</f>
+        <f t="shared" ref="P58:R58" si="42">IF(P27=0,"",P27)</f>
         <v/>
       </c>
       <c r="Q58" s="90" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="R58" s="90">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0.6</v>
       </c>
       <c r="U58" s="158" t="s">
         <v>480</v>
       </c>
       <c r="V58" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C27,3)&amp;" "&amp;AC27</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat OIL Oil boiler condensing.HeatHotwater</v>
       </c>
       <c r="W58" s="47" t="s">
@@ -18542,81 +18523,81 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSSOL_01_EBkp</v>
       </c>
       <c r="B59" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat SOL Solar collector with electric backup.HeatHotwater</v>
       </c>
       <c r="C59" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMELC, COMSOL</v>
       </c>
       <c r="D59" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E59" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F59" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.76259999999999994</v>
       </c>
       <c r="G59" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.965853658536588</v>
       </c>
       <c r="H59" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I59" s="88">
-        <f t="shared" ref="I59:O59" si="40">I28</f>
+        <f t="shared" ref="I59:O59" si="43">I28</f>
         <v>2019</v>
       </c>
       <c r="J59" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>964.81651376146999</v>
       </c>
       <c r="K59" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>185</v>
       </c>
       <c r="L59" s="89">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0.01</v>
       </c>
       <c r="M59" s="88">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N59" s="68">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O59" s="87">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0.16</v>
       </c>
       <c r="P59" s="90" t="str">
-        <f t="shared" ref="P59:R59" si="41">IF(P28=0,"",P28)</f>
+        <f t="shared" ref="P59:R59" si="44">IF(P28=0,"",P28)</f>
         <v/>
       </c>
       <c r="Q59" s="90">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.68</v>
       </c>
       <c r="R59" s="90">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.6</v>
       </c>
       <c r="U59" s="158" t="s">
         <v>481</v>
       </c>
       <c r="V59" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C28,3)&amp;" "&amp;AC28</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat SOL Solar collector with electric backup.HeatHotwater</v>
       </c>
       <c r="W59" s="47" t="s">
@@ -18629,81 +18610,81 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSSOL_02_DBkp</v>
       </c>
       <c r="B60" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat SOL Solar collector with diesel backup.HeatHotwater</v>
       </c>
       <c r="C60" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMOIL, COMSOL</v>
       </c>
       <c r="D60" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E60" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F60" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.76259999999999994</v>
       </c>
       <c r="G60" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.59268292682926904</v>
       </c>
       <c r="H60" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I60" s="88">
-        <f t="shared" ref="I60:O60" si="42">I29</f>
+        <f t="shared" ref="I60:O60" si="45">I29</f>
         <v>2019</v>
       </c>
       <c r="J60" s="82">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>964.81651376146999</v>
       </c>
       <c r="K60" s="82">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>185</v>
       </c>
       <c r="L60" s="89">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.01</v>
       </c>
       <c r="M60" s="88">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="N60" s="68">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O60" s="87">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.16</v>
       </c>
       <c r="P60" s="90" t="str">
-        <f t="shared" ref="P60:R60" si="43">IF(P29=0,"",P29)</f>
+        <f t="shared" ref="P60:R60" si="46">IF(P29=0,"",P29)</f>
         <v/>
       </c>
       <c r="Q60" s="90">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.71</v>
       </c>
       <c r="R60" s="90">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.6</v>
       </c>
       <c r="U60" s="158" t="s">
         <v>518</v>
       </c>
       <c r="V60" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C29,3)&amp;" "&amp;AC29</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat SOL Solar collector with diesel backup.HeatHotwater</v>
       </c>
       <c r="W60" s="47" t="s">
@@ -18716,81 +18697,81 @@
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSSOL_03_GBkp</v>
       </c>
       <c r="B61" s="67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat SOL Solar collector with gas backup.HeatHotwater</v>
       </c>
       <c r="C61" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMGAS, COMSOL</v>
       </c>
       <c r="D61" s="86" t="s">
         <v>327</v>
       </c>
       <c r="E61" s="87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F61" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.79049999999999998</v>
       </c>
       <c r="G61" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.59268292682926904</v>
       </c>
       <c r="H61" s="87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I61" s="88">
-        <f t="shared" ref="I61:O61" si="44">I30</f>
+        <f t="shared" ref="I61:O61" si="47">I30</f>
         <v>2019</v>
       </c>
       <c r="J61" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>964.81651376146999</v>
       </c>
       <c r="K61" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>185</v>
       </c>
       <c r="L61" s="89">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>0.01</v>
       </c>
       <c r="M61" s="88">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>20</v>
       </c>
       <c r="N61" s="68">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O61" s="87">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>0.16</v>
       </c>
       <c r="P61" s="90" t="str">
-        <f t="shared" ref="P61:R61" si="45">IF(P30=0,"",P30)</f>
+        <f t="shared" ref="P61:R61" si="48">IF(P30=0,"",P30)</f>
         <v/>
       </c>
       <c r="Q61" s="90">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.68</v>
       </c>
       <c r="R61" s="90">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.6</v>
       </c>
       <c r="U61" s="158" t="s">
         <v>519</v>
       </c>
       <c r="V61" s="47" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C30,3)&amp;" "&amp;AC30</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat SOL Solar collector with gas backup.HeatHotwater</v>
       </c>
       <c r="W61" s="47" t="s">
@@ -18803,74 +18784,74 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" s="91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>CHPSBIO_01_DBoi</v>
       </c>
       <c r="B62" s="73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>New commercial - PS Space Heat BIO Wood-pellets boiler.HeatHotwater</v>
       </c>
       <c r="C62" s="73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>COMBIO</v>
       </c>
       <c r="D62" s="91" t="s">
         <v>327</v>
       </c>
       <c r="E62" s="97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F62" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.79049999999999998</v>
       </c>
       <c r="G62" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.37619999999999998</v>
       </c>
       <c r="H62" s="92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I62" s="93">
-        <f t="shared" ref="I62:O62" si="46">I31</f>
+        <f t="shared" ref="I62:O62" si="49">I31</f>
         <v>2019</v>
       </c>
       <c r="J62" s="94">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>300</v>
       </c>
       <c r="K62" s="94">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>2</v>
       </c>
       <c r="L62" s="95">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.01</v>
       </c>
       <c r="M62" s="93">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>20</v>
       </c>
       <c r="N62" s="74">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>31.536000000000001</v>
       </c>
       <c r="O62" s="92">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.16</v>
       </c>
       <c r="P62" s="96" t="str">
-        <f t="shared" ref="P62:R62" si="47">IF(P31=0,"",P31)</f>
+        <f t="shared" ref="P62:R62" si="50">IF(P31=0,"",P31)</f>
         <v/>
       </c>
       <c r="Q62" s="96" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="R62" s="96">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0.6</v>
       </c>
       <c r="T62" s="97"/>
@@ -18878,7 +18859,7 @@
         <v>482</v>
       </c>
       <c r="V62" s="97" t="str">
-        <f>"New commercial - PS Space Heat "&amp;RIGHT(C31,3)&amp;" "&amp;AC31</f>
+        <f t="shared" si="10"/>
         <v>New commercial - PS Space Heat BIO Wood-pellets boiler.HeatHotwater</v>
       </c>
       <c r="W62" s="97" t="s">
@@ -19065,11 +19046,11 @@
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="217" t="str">
-        <f t="shared" ref="A69:A72" si="48">U69</f>
+        <f t="shared" ref="A69:A72" si="51">U69</f>
         <v>CHCSGH2_01_Boi</v>
       </c>
       <c r="B69" s="218" t="str">
-        <f t="shared" ref="B69:B72" si="49">V69</f>
+        <f t="shared" ref="B69:B72" si="52">V69</f>
         <v>New commercial - CS Space Heat H2G Gaseous hydrogen boiler</v>
       </c>
       <c r="C69" s="219" t="s">
@@ -19098,9 +19079,8 @@
         <v>0.19996427044383505</v>
       </c>
       <c r="L69" s="224"/>
-      <c r="M69" s="221" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="M69" s="242">
+        <v>20</v>
       </c>
       <c r="N69" s="225">
         <f>G90</f>
@@ -19137,11 +19117,11 @@
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="86" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>CHCSGH2_02_DBoi</v>
       </c>
       <c r="B70" s="67" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>New commercial - CS Space Heat H2G Gaseous hydrogen boiler.HeatHotwater</v>
       </c>
       <c r="C70" s="159" t="s">
@@ -19173,9 +19153,9 @@
         <v>0.19996427044383505</v>
       </c>
       <c r="L70" s="89"/>
-      <c r="M70" s="88" t="e">
+      <c r="M70" s="238">
         <f>M69</f>
-        <v>#REF!</v>
+        <v>20</v>
       </c>
       <c r="N70" s="68">
         <f>N69</f>
@@ -19219,11 +19199,11 @@
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" s="86" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>CHCSGH2_03_HP</v>
       </c>
       <c r="B71" s="67" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>New commercial - CS Space Heat H2G Gaseous hydrogen air heat pump</v>
       </c>
       <c r="C71" s="159" t="s">
@@ -19252,9 +19232,8 @@
         <v>0.32856874241555639</v>
       </c>
       <c r="L71" s="89"/>
-      <c r="M71" s="88" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="M71" s="238">
+        <v>20</v>
       </c>
       <c r="N71" s="68">
         <f>G96</f>
@@ -19298,11 +19277,11 @@
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="91" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>CHCSGH2_04_DHP</v>
       </c>
       <c r="B72" s="73" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>New commercial - CS Space Heat H2G Gaseous hydrogen heat pump.HeatCool</v>
       </c>
       <c r="C72" s="214" t="s">
@@ -19334,9 +19313,9 @@
         <v>0.32856874241555639</v>
       </c>
       <c r="L72" s="95"/>
-      <c r="M72" s="93" t="e">
+      <c r="M72" s="243">
         <f>M71</f>
-        <v>#REF!</v>
+        <v>20</v>
       </c>
       <c r="N72" s="74">
         <f>N71</f>
@@ -19598,73 +19577,73 @@
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" s="217" t="str">
-        <f t="shared" ref="A77:A80" si="50">U77</f>
+        <f t="shared" ref="A77:A80" si="53">U77</f>
         <v>CHPSGH2_01_Boi</v>
       </c>
       <c r="B77" s="218" t="str">
-        <f t="shared" ref="B77:B80" si="51">V77</f>
+        <f t="shared" ref="B77:B80" si="54">V77</f>
         <v>New commercial - PS Space Heat H2G Gaseous hydrogen boiler</v>
       </c>
       <c r="C77" s="219" t="s">
         <v>621</v>
       </c>
-      <c r="D77" s="217" t="s">
-        <v>319</v>
+      <c r="D77" s="177" t="s">
+        <v>320</v>
       </c>
       <c r="E77" s="220">
         <f>IF(E69=0,"",E69)</f>
         <v>0.9</v>
       </c>
       <c r="F77" s="220" t="str">
-        <f t="shared" ref="F77:R77" si="52">IF(F69=0,"",F69)</f>
+        <f t="shared" ref="F77:R77" si="55">IF(F69=0,"",F69)</f>
         <v/>
       </c>
       <c r="G77" s="220" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="H77" s="220" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="I77" s="221">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>2030</v>
       </c>
       <c r="J77" s="222">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>1.9996427044383505</v>
       </c>
       <c r="K77" s="223">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0.19996427044383505</v>
       </c>
       <c r="L77" s="224" t="str">
-        <f t="shared" si="52"/>
-        <v/>
-      </c>
-      <c r="M77" s="221" t="e">
-        <f t="shared" si="52"/>
-        <v>#REF!</v>
+        <f t="shared" si="55"/>
+        <v/>
+      </c>
+      <c r="M77" s="242">
+        <f t="shared" si="55"/>
+        <v>20</v>
       </c>
       <c r="N77" s="225">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>1</v>
       </c>
       <c r="O77" s="220">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0.15</v>
       </c>
       <c r="P77" s="226" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="Q77" s="226" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="R77" s="226" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="T77" s="228" t="s">
@@ -19692,73 +19671,73 @@
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="86" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>CHPSGH2_02_DBoi</v>
       </c>
       <c r="B78" s="67" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>New commercial - PS Space Heat H2G Gaseous hydrogen boiler.HeatHotwater</v>
       </c>
       <c r="C78" s="159" t="s">
         <v>621</v>
       </c>
-      <c r="D78" s="86" t="s">
-        <v>325</v>
+      <c r="D78" s="244" t="s">
+        <v>327</v>
       </c>
       <c r="E78" s="87" t="str">
-        <f t="shared" ref="E78:R78" si="53">IF(E70=0,"",E70)</f>
+        <f t="shared" ref="E78:R78" si="56">IF(E70=0,"",E70)</f>
         <v/>
       </c>
       <c r="F78" s="87">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.9</v>
       </c>
       <c r="G78" s="213">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.4564421741298722</v>
       </c>
       <c r="H78" s="87" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="I78" s="88">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>2030</v>
       </c>
       <c r="J78" s="82">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1.9996427044383505</v>
       </c>
       <c r="K78" s="82">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.19996427044383505</v>
       </c>
       <c r="L78" s="89" t="str">
-        <f t="shared" si="53"/>
-        <v/>
-      </c>
-      <c r="M78" s="88" t="e">
-        <f t="shared" si="53"/>
-        <v>#REF!</v>
+        <f t="shared" si="56"/>
+        <v/>
+      </c>
+      <c r="M78" s="238">
+        <f t="shared" si="56"/>
+        <v>20</v>
       </c>
       <c r="N78" s="68">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1</v>
       </c>
       <c r="O78" s="87">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.15</v>
       </c>
       <c r="P78" s="90" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="Q78" s="90" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="R78" s="90">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.6</v>
       </c>
       <c r="T78" s="85"/>
@@ -19784,73 +19763,73 @@
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="86" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>CHPSGH2_03_HP</v>
       </c>
       <c r="B79" s="67" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>New commercial - PS Space Heat H2G Gaseous hydrogen air heat pump</v>
       </c>
       <c r="C79" s="159" t="s">
         <v>708</v>
       </c>
-      <c r="D79" s="86" t="s">
-        <v>319</v>
+      <c r="D79" s="244" t="s">
+        <v>320</v>
       </c>
       <c r="E79" s="87">
-        <f t="shared" ref="E79:R79" si="54">IF(E71=0,"",E71)</f>
+        <f t="shared" ref="E79:R79" si="57">IF(E71=0,"",E71)</f>
         <v>0.93</v>
       </c>
       <c r="F79" s="87" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="G79" s="87" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="H79" s="87" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="I79" s="88">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>2030</v>
       </c>
       <c r="J79" s="82">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>5.4761457069259398</v>
       </c>
       <c r="K79" s="215">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.32856874241555639</v>
       </c>
       <c r="L79" s="89" t="str">
-        <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="M79" s="88" t="e">
-        <f t="shared" si="54"/>
-        <v>#REF!</v>
+        <f t="shared" si="57"/>
+        <v/>
+      </c>
+      <c r="M79" s="238">
+        <f t="shared" si="57"/>
+        <v>20</v>
       </c>
       <c r="N79" s="68">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>1</v>
       </c>
       <c r="O79" s="87">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.15</v>
       </c>
       <c r="P79" s="90">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.42857142857142899</v>
       </c>
       <c r="Q79" s="90" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="R79" s="90" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="T79" s="85"/>
@@ -19876,73 +19855,73 @@
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="91" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>CHPSGH2_04_DHP</v>
       </c>
       <c r="B80" s="73" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>New commercial - PS Space Heat H2G Gaseous hydrogen heat pump.HeatCool</v>
       </c>
       <c r="C80" s="214" t="s">
         <v>708</v>
       </c>
-      <c r="D80" s="91" t="s">
-        <v>324</v>
+      <c r="D80" s="245" t="s">
+        <v>326</v>
       </c>
       <c r="E80" s="92" t="str">
-        <f t="shared" ref="E80:R80" si="55">IF(E72=0,"",E72)</f>
+        <f t="shared" ref="E80:R80" si="58">IF(E72=0,"",E72)</f>
         <v/>
       </c>
       <c r="F80" s="92">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.93</v>
       </c>
       <c r="G80" s="92" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="H80" s="92">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="I80" s="93">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2030</v>
       </c>
       <c r="J80" s="94">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>5.4761457069259398</v>
       </c>
       <c r="K80" s="94">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.32856874241555639</v>
       </c>
       <c r="L80" s="95" t="str">
-        <f t="shared" si="55"/>
-        <v/>
-      </c>
-      <c r="M80" s="93" t="e">
-        <f t="shared" si="55"/>
-        <v>#REF!</v>
+        <f t="shared" si="58"/>
+        <v/>
+      </c>
+      <c r="M80" s="243">
+        <f t="shared" si="58"/>
+        <v>20</v>
       </c>
       <c r="N80" s="74">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="O80" s="92">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.15</v>
       </c>
       <c r="P80" s="96">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.42857142857142899</v>
       </c>
       <c r="Q80" s="96" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="R80" s="96" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="T80" s="97"/>
@@ -20747,8 +20726,8 @@
   </sheetPr>
   <dimension ref="A1:V113"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30184,9 +30163,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30336,19 +30318,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A420273B-2C8D-4520-9FDE-EF20D51299FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A07C550-9056-4674-9B3B-CB67924D4B57}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30372,9 +30350,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A07C550-9056-4674-9B3B-CB67924D4B57}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A420273B-2C8D-4520-9FDE-EF20D51299FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>